<commit_message>
40 pin FPC tester sent to fabrication
</commit_message>
<xml_diff>
--- a/hardware/extension-40_to_PCB_test/BOM.xlsx
+++ b/hardware/extension-40_to_PCB_test/BOM.xlsx
@@ -16,6 +16,41 @@
   <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <webPublishing allowPng="1" css="0" characterSet="UTF-8"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10" count="10">
+  <si>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>JLCPCB Part #</t>
+  </si>
+  <si>
+    <t>R_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>LED_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>FH1240S05SH55</t>
+  </si>
+  <si>
+    <t>ED078KH6</t>
+  </si>
+  <si>
+    <t>C202114</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -76,106 +111,170 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" style="0" width="12.284975961538462" customWidth="1"/>
-    <col min="2" max="2" style="0" width="19.28455528846154" customWidth="1"/>
+    <col min="2" max="2" style="0" width="23.855709134615388" customWidth="1"/>
     <col min="3" max="3" style="0" width="17.57037259615385" customWidth="1"/>
     <col min="4" max="4" style="0" width="13.284915865384617" customWidth="1"/>
     <col min="5" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13.5">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Designator</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Footprint</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Comments</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>JLCPCB Part #</t>
-        </is>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="13.5">
       <c r="A2" t="inlineStr">
         <is>
-          <t>J1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>FH1233S05SH55</t>
-        </is>
+          <t>R8,R7,R22,R14,R9,R4,R1,R20,R21,R12,R19,R11,R18,R6,R3,R23,R2,R10,R16,R15,R13,R17,R5</t>
+        </is>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>XF2M-3315-1A</t>
+          <t>2.4k</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>C597986</t>
+          <t>C22940</t>
         </is>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13.5">
       <c r="A3" t="inlineStr">
         <is>
-          <t>U1,U3</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>X05A20H34G</t>
-        </is>
+          <t>D7,D1,D15,D11,D14,D8,D9,D13,D4,D12,D5,D2,D0,D6,D10,D3</t>
+        </is>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ED060XC5</t>
+          <t>LED GREEN</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>C528053</t>
+          <t>C2297</t>
         </is>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13.5">
       <c r="A4" t="inlineStr">
         <is>
-          <t>U2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>FH1240S05SH55</t>
-        </is>
+          <t>CKV1,XSTL1,OE1,STV1,EP_MODE1,XCL1,LEH1</t>
+        </is>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ED078KH6</t>
+          <t>LED RED</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>C202114</t>
+          <t>C84256</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="13.5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>R25,R24</t>
+        </is>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>33k</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>C4216</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13.5">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>XKTF005-SD</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>XKTF-005</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>C2689687</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="13.5">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>U1</t>
+        </is>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="13.5">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>RN1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SMT_F392JTCE_UNR_SD-pullup</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>R_arr 35K Ω</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>C425297</t>
         </is>
       </c>
     </row>

</xml_diff>